<commit_message>
parsed new data sets. implemented new data strategy so we can have entries and exits.
</commit_message>
<xml_diff>
--- a/data/Ridership_June2013.xlsx
+++ b/data/Ridership_June2013.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="4" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="371" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
+    <workbookView activeTab="4" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="439" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
     <sheet name="Weekday OD" sheetId="1" state="visible" r:id="rId2"/>
@@ -23,21 +23,26 @@
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Titles" vbProcedure="false">'Weekday OD'!$A:$A</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Titles" vbProcedure="false">'Weekday OD'!$A:$A</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Titles_0" vbProcedure="false">'Weekday OD'!$A:$A</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Titles_0_0" vbProcedure="false">'Weekday OD'!$A:$A</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm.Print_Area" vbProcedure="false">'Saturday OD'!$A$1:$AT$47</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm.Print_Area_0" vbProcedure="false">'Saturday OD'!$A$1:$AT$47</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm.Print_Area_0_0" vbProcedure="false">'Saturday OD'!$A$1:$AT$47</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm.Print_Titles" vbProcedure="false">'Saturday OD'!$A:$A</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm.Print_Titles_0" vbProcedure="false">'Saturday OD'!$A:$A</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm.Print_Titles_0_0" vbProcedure="false">'Saturday OD'!$A:$A</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm.Print_Area" vbProcedure="false">'Sunday OD'!$A$1:$AT$47</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm.Print_Area_0" vbProcedure="false">'Sunday OD'!$A$1:$AT$47</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm.Print_Area_0_0" vbProcedure="false">'Sunday OD'!$A$1:$AT$47</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm.Print_Titles" vbProcedure="false">'Sunday OD'!$A:$A</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm.Print_Titles_0" vbProcedure="false">'Sunday OD'!$A:$A</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm.Print_Titles_0_0" vbProcedure="false">'Sunday OD'!$A:$A</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="761" uniqueCount="218">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="626" uniqueCount="166">
   <si>
     <t>Exit stations</t>
   </si>
@@ -246,16 +251,7 @@
     <t>gtfs_longitude</t>
   </si>
   <si>
-    <t>address</t>
-  </si>
-  <si>
     <t>city</t>
-  </si>
-  <si>
-    <t>county</t>
-  </si>
-  <si>
-    <t>state</t>
   </si>
   <si>
     <t>zipcode</t>
@@ -270,16 +266,7 @@
     <t>12TH</t>
   </si>
   <si>
-    <t>1245 Broadway</t>
-  </si>
-  <si>
     <t>Oakland</t>
-  </si>
-  <si>
-    <t>alameda</t>
-  </si>
-  <si>
-    <t>CA</t>
   </si>
   <si>
     <t>16th St. Mission</t>
@@ -288,13 +275,7 @@
     <t>16TH</t>
   </si>
   <si>
-    <t>2000 Mission Street</t>
-  </si>
-  <si>
     <t>San Francisco</t>
-  </si>
-  <si>
-    <t>sanfrancisco</t>
   </si>
   <si>
     <t>19th St. Oakland</t>
@@ -303,25 +284,16 @@
     <t>19TH</t>
   </si>
   <si>
-    <t>1900 Broadway</t>
-  </si>
-  <si>
     <t>24th St. Mission</t>
   </si>
   <si>
     <t>24TH</t>
   </si>
   <si>
-    <t>2800 Mission Street</t>
-  </si>
-  <si>
     <t>Ashby</t>
   </si>
   <si>
     <t>ASHB</t>
-  </si>
-  <si>
-    <t>3100 Adeline Street</t>
   </si>
   <si>
     <t>Berkeley</t>
@@ -333,9 +305,6 @@
     <t>BAYF</t>
   </si>
   <si>
-    <t>15242 Hesperian Blvd.</t>
-  </si>
-  <si>
     <t>San Leandro</t>
   </si>
   <si>
@@ -345,16 +314,10 @@
     <t>CAST</t>
   </si>
   <si>
-    <t>3301 Norbridge Dr.</t>
-  </si>
-  <si>
     <t>Balboa Park</t>
   </si>
   <si>
     <t>BALB</t>
-  </si>
-  <si>
-    <t>401 Geneva Avenue</t>
   </si>
   <si>
     <t>Coliseum/Oakland Airport</t>
@@ -363,19 +326,10 @@
     <t>COLS</t>
   </si>
   <si>
-    <t>7200 San Leandro St.</t>
-  </si>
-  <si>
     <t>Colma</t>
   </si>
   <si>
     <t>COLM</t>
-  </si>
-  <si>
-    <t>365 D Street</t>
-  </si>
-  <si>
-    <t>sanmateo</t>
   </si>
   <si>
     <t>Concord</t>
@@ -384,19 +338,10 @@
     <t>CONC</t>
   </si>
   <si>
-    <t>1451 Oakland Avenue</t>
-  </si>
-  <si>
-    <t>contracosta</t>
-  </si>
-  <si>
     <t>Daly City</t>
   </si>
   <si>
     <t>DALY</t>
-  </si>
-  <si>
-    <t>500 John Daly Blvd.</t>
   </si>
   <si>
     <t>Civic Center/UN Plaza</t>
@@ -405,25 +350,16 @@
     <t>CIVC</t>
   </si>
   <si>
-    <t>1150 Market Street</t>
-  </si>
-  <si>
     <t>Downtown Berkeley</t>
   </si>
   <si>
     <t>DBRK</t>
   </si>
   <si>
-    <t>2160 Shattuck Avenue</t>
-  </si>
-  <si>
     <t>Dublin/Pleasanton</t>
   </si>
   <si>
     <t>DUBL</t>
-  </si>
-  <si>
-    <t>5801 Owens Dr.</t>
   </si>
   <si>
     <t>Pleasanton</t>
@@ -435,16 +371,10 @@
     <t>EMBR</t>
   </si>
   <si>
-    <t>298 Market Street</t>
-  </si>
-  <si>
     <t>El Cerrito del Norte</t>
   </si>
   <si>
     <t>DELN</t>
-  </si>
-  <si>
-    <t>6400 Cutting Blvd.</t>
   </si>
   <si>
     <t>El Cerrito</t>
@@ -456,16 +386,10 @@
     <t>PLZA</t>
   </si>
   <si>
-    <t>6699 Fairmount Avenue</t>
-  </si>
-  <si>
     <t>Fremont</t>
   </si>
   <si>
     <t>FRMT</t>
-  </si>
-  <si>
-    <t>2000 BART Way</t>
   </si>
   <si>
     <t>Fruitvale</t>
@@ -474,16 +398,10 @@
     <t>FTVL</t>
   </si>
   <si>
-    <t>3401 East 12th Street</t>
-  </si>
-  <si>
     <t>Glen Park</t>
   </si>
   <si>
     <t>GLEN</t>
-  </si>
-  <si>
-    <t>2901 Diamond Street</t>
   </si>
   <si>
     <t>Hayward</t>
@@ -492,16 +410,10 @@
     <t>HAYW</t>
   </si>
   <si>
-    <t>699 'B' Street</t>
-  </si>
-  <si>
     <t>Lafayette</t>
   </si>
   <si>
     <t>LAFY</t>
-  </si>
-  <si>
-    <t>3601 Deer Hill Road</t>
   </si>
   <si>
     <t>Lake Merritt</t>
@@ -510,16 +422,10 @@
     <t>LAKE</t>
   </si>
   <si>
-    <t>800 Madison Street</t>
-  </si>
-  <si>
     <t>MacArthur</t>
   </si>
   <si>
     <t>MCAR</t>
-  </si>
-  <si>
-    <t>555 40th Street</t>
   </si>
   <si>
     <t>Millbrae</t>
@@ -528,16 +434,10 @@
     <t>MLBR</t>
   </si>
   <si>
-    <t>200 North Rollins Road</t>
-  </si>
-  <si>
     <t>Montgomery St.</t>
   </si>
   <si>
     <t>MONT</t>
-  </si>
-  <si>
-    <t>598 Market Street</t>
   </si>
   <si>
     <t>North Berkeley</t>
@@ -546,16 +446,10 @@
     <t>NBRK</t>
   </si>
   <si>
-    <t>1750 Sacramento Street</t>
-  </si>
-  <si>
     <t>North Concord/Martinez</t>
   </si>
   <si>
     <t>NCON</t>
-  </si>
-  <si>
-    <t>3700 Port Chicago Highway</t>
   </si>
   <si>
     <t>Orinda</t>
@@ -564,25 +458,16 @@
     <t>ORIN</t>
   </si>
   <si>
-    <t>11 Camino Pablo</t>
-  </si>
-  <si>
     <t>West Oakland</t>
   </si>
   <si>
     <t>WOAK</t>
   </si>
   <si>
-    <t>1451 7th Street</t>
-  </si>
-  <si>
     <t>Pleasant Hill/Contra Costa Centre</t>
   </si>
   <si>
     <t>PHIL</t>
-  </si>
-  <si>
-    <t>1365 Treat Blvd.</t>
   </si>
   <si>
     <t>Walnut Creek</t>
@@ -594,16 +479,10 @@
     <t>POWL</t>
   </si>
   <si>
-    <t>899 Market Street</t>
-  </si>
-  <si>
     <t>Richmond</t>
   </si>
   <si>
     <t>RICH</t>
-  </si>
-  <si>
-    <t>1700 Nevin Avenue</t>
   </si>
   <si>
     <t>Rockridge</t>
@@ -612,16 +491,10 @@
     <t>ROCK</t>
   </si>
   <si>
-    <t>5660 College Avenue</t>
-  </si>
-  <si>
     <t>San Bruno</t>
   </si>
   <si>
     <t>SBRN</t>
-  </si>
-  <si>
-    <t>1151 Huntington Avenue</t>
   </si>
   <si>
     <t>South Hayward</t>
@@ -630,19 +503,10 @@
     <t>SHAY</t>
   </si>
   <si>
-    <t>28601 Dixon Street</t>
-  </si>
-  <si>
     <t>SANL</t>
   </si>
   <si>
-    <t>1401 San Leandro Blvd.</t>
-  </si>
-  <si>
     <t>San Francisco Int'l Airport</t>
-  </si>
-  <si>
-    <t>International Terminal, Level 3</t>
   </si>
   <si>
     <t>South San Francisco</t>
@@ -651,31 +515,19 @@
     <t>SSAN</t>
   </si>
   <si>
-    <t>1333 Mission Road</t>
-  </si>
-  <si>
     <t>Union City</t>
   </si>
   <si>
     <t>UCTY</t>
   </si>
   <si>
-    <t>10 Union Square</t>
-  </si>
-  <si>
     <t>WCRK</t>
-  </si>
-  <si>
-    <t>200 Ygnacio Valley Road</t>
   </si>
   <si>
     <t>West Dublin/Pleasanton</t>
   </si>
   <si>
     <t>WDUB</t>
-  </si>
-  <si>
-    <t>6501 Golden Gate Drive</t>
   </si>
   <si>
     <t>Dublin</t>
@@ -685,9 +537,6 @@
   </si>
   <si>
     <t>PITT</t>
-  </si>
-  <si>
-    <t>1700 West Leland Road</t>
   </si>
   <si>
     <t>Pittsburg</t>
@@ -856,12 +705,12 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="45" min="1" style="0" width="7.79607843137255"/>
-    <col collapsed="false" hidden="false" max="46" min="46" style="1" width="8.8"/>
-    <col collapsed="false" hidden="false" max="47" min="47" style="1" width="9.23529411764706"/>
-    <col collapsed="false" hidden="false" max="49" min="48" style="0" width="9.23529411764706"/>
-    <col collapsed="false" hidden="false" max="50" min="50" style="0" width="8.8"/>
-    <col collapsed="false" hidden="false" max="1025" min="51" style="0" width="9.23529411764706"/>
+    <col collapsed="false" hidden="false" max="45" min="1" style="0" width="7.83137254901961"/>
+    <col collapsed="false" hidden="false" max="46" min="46" style="1" width="8.84705882352941"/>
+    <col collapsed="false" hidden="false" max="47" min="47" style="1" width="9.27843137254902"/>
+    <col collapsed="false" hidden="false" max="49" min="48" style="0" width="9.27843137254902"/>
+    <col collapsed="false" hidden="false" max="50" min="50" style="0" width="8.84705882352941"/>
+    <col collapsed="false" hidden="false" max="1025" min="51" style="0" width="9.27843137254902"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="26.25" outlineLevel="0" r="1">
@@ -7953,12 +7802,12 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="45" min="1" style="0" width="7.79607843137255"/>
-    <col collapsed="false" hidden="false" max="46" min="46" style="1" width="8.8"/>
-    <col collapsed="false" hidden="false" max="47" min="47" style="1" width="9.23529411764706"/>
-    <col collapsed="false" hidden="false" max="49" min="48" style="0" width="9.23529411764706"/>
-    <col collapsed="false" hidden="false" max="50" min="50" style="0" width="8.8"/>
-    <col collapsed="false" hidden="false" max="1025" min="51" style="0" width="9.23529411764706"/>
+    <col collapsed="false" hidden="false" max="45" min="1" style="0" width="7.83137254901961"/>
+    <col collapsed="false" hidden="false" max="46" min="46" style="1" width="8.84705882352941"/>
+    <col collapsed="false" hidden="false" max="47" min="47" style="1" width="9.27843137254902"/>
+    <col collapsed="false" hidden="false" max="49" min="48" style="0" width="9.27843137254902"/>
+    <col collapsed="false" hidden="false" max="50" min="50" style="0" width="8.84705882352941"/>
+    <col collapsed="false" hidden="false" max="1025" min="51" style="0" width="9.27843137254902"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="27" outlineLevel="0" r="1">
@@ -15027,12 +14876,12 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="45" min="1" style="0" width="7.79607843137255"/>
-    <col collapsed="false" hidden="false" max="46" min="46" style="1" width="8.8"/>
-    <col collapsed="false" hidden="false" max="47" min="47" style="1" width="9.23529411764706"/>
-    <col collapsed="false" hidden="false" max="49" min="48" style="0" width="9.23529411764706"/>
-    <col collapsed="false" hidden="false" max="50" min="50" style="0" width="8.8"/>
-    <col collapsed="false" hidden="false" max="1025" min="51" style="0" width="9.23529411764706"/>
+    <col collapsed="false" hidden="false" max="45" min="1" style="0" width="7.83137254901961"/>
+    <col collapsed="false" hidden="false" max="46" min="46" style="1" width="8.84705882352941"/>
+    <col collapsed="false" hidden="false" max="47" min="47" style="1" width="9.27843137254902"/>
+    <col collapsed="false" hidden="false" max="49" min="48" style="0" width="9.27843137254902"/>
+    <col collapsed="false" hidden="false" max="50" min="50" style="0" width="8.84705882352941"/>
+    <col collapsed="false" hidden="false" max="1025" min="51" style="0" width="9.27843137254902"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="26.25" outlineLevel="0" r="1">
@@ -22101,8 +21950,8 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="10" min="1" style="0" width="8.21960784313725"/>
-    <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="8.76470588235294"/>
+    <col collapsed="false" hidden="false" max="10" min="1" style="0" width="8.25882352941177"/>
+    <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="8.8078431372549"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="1">
@@ -23139,15 +22988,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K45"/>
+  <dimension ref="A1:H45"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="L2" activeCellId="0" pane="topLeft" sqref="L2"/>
+      <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="28.9490196078431"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="11.6313725490196"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="29.0941176470588"/>
+    <col collapsed="false" hidden="false" max="5" min="2" style="0" width="11.6941176470588"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="22.521568627451"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="11.6941176470588"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="1">
@@ -23175,25 +23026,16 @@
       <c r="H1" s="0" t="s">
         <v>71</v>
       </c>
-      <c r="I1" s="0" t="s">
-        <v>72</v>
-      </c>
-      <c r="J1" s="0" t="s">
-        <v>73</v>
-      </c>
-      <c r="K1" s="0" t="s">
-        <v>74</v>
-      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="2">
       <c r="A2" s="0" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>12</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="D2" s="0" t="n">
         <v>37.803664</v>
@@ -23202,33 +23044,24 @@
         <v>-122.271604</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>77</v>
-      </c>
-      <c r="G2" s="0" t="s">
-        <v>78</v>
-      </c>
-      <c r="H2" s="0" t="s">
-        <v>79</v>
-      </c>
-      <c r="I2" s="0" t="s">
-        <v>80</v>
-      </c>
-      <c r="J2" s="0" t="n">
+        <v>74</v>
+      </c>
+      <c r="G2" s="0" t="n">
         <v>94612</v>
       </c>
-      <c r="K2" s="0" t="n">
+      <c r="H2" s="0" t="n">
         <v>8</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="3">
       <c r="A3" s="0" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>16</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="D3" s="0" t="n">
         <v>37.765062</v>
@@ -23237,33 +23070,24 @@
         <v>-122.419694</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>83</v>
-      </c>
-      <c r="G3" s="0" t="s">
-        <v>84</v>
-      </c>
-      <c r="H3" s="0" t="s">
-        <v>85</v>
-      </c>
-      <c r="I3" s="0" t="s">
-        <v>80</v>
-      </c>
-      <c r="J3" s="0" t="n">
+        <v>77</v>
+      </c>
+      <c r="G3" s="0" t="n">
         <v>94110</v>
       </c>
-      <c r="K3" s="0" t="n">
+      <c r="H3" s="0" t="n">
         <v>29</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="4">
       <c r="A4" s="0" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>19</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="D4" s="0" t="n">
         <v>37.80787</v>
@@ -23272,33 +23096,24 @@
         <v>-122.269029</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>88</v>
-      </c>
-      <c r="G4" s="0" t="s">
-        <v>78</v>
-      </c>
-      <c r="H4" s="0" t="s">
-        <v>79</v>
-      </c>
-      <c r="I4" s="0" t="s">
-        <v>80</v>
-      </c>
-      <c r="J4" s="0" t="n">
+        <v>74</v>
+      </c>
+      <c r="G4" s="0" t="n">
         <v>94612</v>
       </c>
-      <c r="K4" s="0" t="n">
+      <c r="H4" s="0" t="n">
         <v>7</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="5">
       <c r="A5" s="0" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>24</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="D5" s="0" t="n">
         <v>37.752254</v>
@@ -23307,33 +23122,24 @@
         <v>-122.418466</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>91</v>
-      </c>
-      <c r="G5" s="0" t="s">
-        <v>84</v>
-      </c>
-      <c r="H5" s="0" t="s">
-        <v>85</v>
-      </c>
-      <c r="I5" s="0" t="s">
-        <v>80</v>
-      </c>
-      <c r="J5" s="0" t="n">
+        <v>77</v>
+      </c>
+      <c r="G5" s="0" t="n">
         <v>94110</v>
       </c>
-      <c r="K5" s="0" t="n">
+      <c r="H5" s="0" t="n">
         <v>30</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="6">
       <c r="A6" s="0" t="s">
-        <v>92</v>
+        <v>82</v>
       </c>
       <c r="B6" s="0" t="s">
         <v>8</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="D6" s="0" t="n">
         <v>37.853024</v>
@@ -23342,33 +23148,24 @@
         <v>-122.26978</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>94</v>
-      </c>
-      <c r="G6" s="0" t="s">
-        <v>95</v>
-      </c>
-      <c r="H6" s="0" t="s">
-        <v>79</v>
-      </c>
-      <c r="I6" s="0" t="s">
-        <v>80</v>
-      </c>
-      <c r="J6" s="0" t="n">
+        <v>84</v>
+      </c>
+      <c r="G6" s="0" t="n">
         <v>94703</v>
       </c>
-      <c r="K6" s="0" t="n">
+      <c r="H6" s="0" t="n">
         <v>5</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="7">
       <c r="A7" s="0" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
       <c r="B7" s="0" t="s">
         <v>14</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>97</v>
+        <v>86</v>
       </c>
       <c r="D7" s="0" t="n">
         <v>37.697185</v>
@@ -23377,33 +23174,24 @@
         <v>-122.126871</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>98</v>
-      </c>
-      <c r="G7" s="0" t="s">
-        <v>99</v>
-      </c>
-      <c r="H7" s="0" t="s">
-        <v>79</v>
-      </c>
-      <c r="I7" s="0" t="s">
-        <v>80</v>
-      </c>
-      <c r="J7" s="0" t="n">
+        <v>87</v>
+      </c>
+      <c r="G7" s="0" t="n">
         <v>94578</v>
       </c>
-      <c r="K7" s="0" t="n">
+      <c r="H7" s="0" t="n">
         <v>13</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="8">
       <c r="A8" s="0" t="s">
-        <v>100</v>
+        <v>88</v>
       </c>
       <c r="B8" s="0" t="s">
         <v>7</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>101</v>
+        <v>89</v>
       </c>
       <c r="D8" s="0" t="n">
         <v>37.690754</v>
@@ -23412,33 +23200,24 @@
         <v>-122.075567</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>102</v>
-      </c>
-      <c r="G8" s="0" t="s">
-        <v>100</v>
-      </c>
-      <c r="H8" s="0" t="s">
-        <v>79</v>
-      </c>
-      <c r="I8" s="0" t="s">
-        <v>80</v>
-      </c>
-      <c r="J8" s="0" t="n">
+        <v>88</v>
+      </c>
+      <c r="G8" s="0" t="n">
         <v>94546</v>
       </c>
-      <c r="K8" s="0" t="n">
+      <c r="H8" s="0" t="n">
         <v>4</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="9">
       <c r="A9" s="0" t="s">
-        <v>103</v>
+        <v>90</v>
       </c>
       <c r="B9" s="0" t="s">
         <v>31</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>104</v>
+        <v>91</v>
       </c>
       <c r="D9" s="0" t="n">
         <v>37.72198087</v>
@@ -23447,33 +23226,24 @@
         <v>-122.4474142</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>105</v>
-      </c>
-      <c r="G9" s="0" t="s">
-        <v>84</v>
-      </c>
-      <c r="H9" s="0" t="s">
-        <v>85</v>
-      </c>
-      <c r="I9" s="0" t="s">
-        <v>80</v>
-      </c>
-      <c r="J9" s="0" t="n">
+        <v>77</v>
+      </c>
+      <c r="G9" s="0" t="n">
         <v>94112</v>
       </c>
-      <c r="K9" s="0" t="n">
+      <c r="H9" s="0" t="n">
         <v>32</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="10">
       <c r="A10" s="0" t="s">
-        <v>106</v>
+        <v>92</v>
       </c>
       <c r="B10" s="0" t="s">
         <v>29</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>107</v>
+        <v>93</v>
       </c>
       <c r="D10" s="0" t="n">
         <v>37.754006</v>
@@ -23482,33 +23252,24 @@
         <v>-122.197273</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>108</v>
-      </c>
-      <c r="G10" s="0" t="s">
-        <v>78</v>
-      </c>
-      <c r="H10" s="0" t="s">
-        <v>79</v>
-      </c>
-      <c r="I10" s="0" t="s">
-        <v>80</v>
-      </c>
-      <c r="J10" s="0" t="n">
+        <v>74</v>
+      </c>
+      <c r="G10" s="0" t="n">
         <v>94621</v>
       </c>
-      <c r="K10" s="0" t="n">
+      <c r="H10" s="0" t="n">
         <v>28</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="11">
       <c r="A11" s="0" t="s">
-        <v>109</v>
+        <v>94</v>
       </c>
       <c r="B11" s="0" t="s">
         <v>12</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>110</v>
+        <v>95</v>
       </c>
       <c r="D11" s="0" t="n">
         <v>37.684638</v>
@@ -23517,33 +23278,24 @@
         <v>-122.466233</v>
       </c>
       <c r="F11" s="0" t="s">
-        <v>111</v>
-      </c>
-      <c r="G11" s="0" t="s">
-        <v>109</v>
-      </c>
-      <c r="H11" s="0" t="s">
-        <v>112</v>
-      </c>
-      <c r="I11" s="0" t="s">
-        <v>80</v>
-      </c>
-      <c r="J11" s="0" t="n">
+        <v>94</v>
+      </c>
+      <c r="G11" s="0" t="n">
         <v>94014</v>
       </c>
-      <c r="K11" s="0" t="n">
+      <c r="H11" s="0" t="n">
         <v>11</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="12">
       <c r="A12" s="0" t="s">
-        <v>113</v>
+        <v>96</v>
       </c>
       <c r="B12" s="0" t="s">
         <v>33</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>114</v>
+        <v>97</v>
       </c>
       <c r="D12" s="0" t="n">
         <v>37.973737</v>
@@ -23552,33 +23304,24 @@
         <v>-122.029095</v>
       </c>
       <c r="F12" s="0" t="s">
-        <v>115</v>
-      </c>
-      <c r="G12" s="0" t="s">
-        <v>113</v>
-      </c>
-      <c r="H12" s="0" t="s">
-        <v>116</v>
-      </c>
-      <c r="I12" s="0" t="s">
-        <v>80</v>
-      </c>
-      <c r="J12" s="0" t="n">
+        <v>96</v>
+      </c>
+      <c r="G12" s="0" t="n">
         <v>94520</v>
       </c>
-      <c r="K12" s="0" t="n">
+      <c r="H12" s="0" t="n">
         <v>34</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="13">
       <c r="A13" s="0" t="s">
-        <v>117</v>
+        <v>98</v>
       </c>
       <c r="B13" s="0" t="s">
         <v>19</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>118</v>
+        <v>99</v>
       </c>
       <c r="D13" s="0" t="n">
         <v>37.70612055</v>
@@ -23587,33 +23330,24 @@
         <v>-122.4690807</v>
       </c>
       <c r="F13" s="0" t="s">
-        <v>119</v>
-      </c>
-      <c r="G13" s="0" t="s">
-        <v>117</v>
-      </c>
-      <c r="H13" s="0" t="s">
-        <v>112</v>
-      </c>
-      <c r="I13" s="0" t="s">
-        <v>80</v>
-      </c>
-      <c r="J13" s="0" t="n">
+        <v>98</v>
+      </c>
+      <c r="G13" s="0" t="n">
         <v>94014</v>
       </c>
-      <c r="K13" s="0" t="n">
+      <c r="H13" s="0" t="n">
         <v>18</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="14">
       <c r="A14" s="0" t="s">
-        <v>120</v>
+        <v>100</v>
       </c>
       <c r="B14" s="0" t="s">
         <v>34</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>121</v>
+        <v>101</v>
       </c>
       <c r="D14" s="0" t="n">
         <v>37.779528</v>
@@ -23622,33 +23356,24 @@
         <v>-122.413756</v>
       </c>
       <c r="F14" s="0" t="s">
-        <v>122</v>
-      </c>
-      <c r="G14" s="0" t="s">
-        <v>84</v>
-      </c>
-      <c r="H14" s="0" t="s">
-        <v>85</v>
-      </c>
-      <c r="I14" s="0" t="s">
-        <v>80</v>
-      </c>
-      <c r="J14" s="0" t="n">
+        <v>77</v>
+      </c>
+      <c r="G14" s="0" t="n">
         <v>94102</v>
       </c>
-      <c r="K14" s="0" t="n">
+      <c r="H14" s="0" t="n">
         <v>35</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="15">
       <c r="A15" s="0" t="s">
-        <v>123</v>
+        <v>102</v>
       </c>
       <c r="B15" s="0" t="s">
         <v>32</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>124</v>
+        <v>103</v>
       </c>
       <c r="D15" s="0" t="n">
         <v>37.869867</v>
@@ -23657,33 +23382,24 @@
         <v>-122.268045</v>
       </c>
       <c r="F15" s="0" t="s">
-        <v>125</v>
-      </c>
-      <c r="G15" s="0" t="s">
-        <v>95</v>
-      </c>
-      <c r="H15" s="0" t="s">
-        <v>79</v>
-      </c>
-      <c r="I15" s="0" t="s">
-        <v>80</v>
-      </c>
-      <c r="J15" s="0" t="n">
+        <v>84</v>
+      </c>
+      <c r="G15" s="0" t="n">
         <v>94704</v>
       </c>
-      <c r="K15" s="0" t="n">
+      <c r="H15" s="0" t="n">
         <v>33</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="16">
       <c r="A16" s="0" t="s">
-        <v>126</v>
+        <v>104</v>
       </c>
       <c r="B16" s="0" t="s">
         <v>35</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>127</v>
+        <v>105</v>
       </c>
       <c r="D16" s="0" t="n">
         <v>37.701695</v>
@@ -23692,33 +23408,24 @@
         <v>-121.900367</v>
       </c>
       <c r="F16" s="0" t="s">
-        <v>128</v>
-      </c>
-      <c r="G16" s="0" t="s">
-        <v>129</v>
-      </c>
-      <c r="H16" s="0" t="s">
-        <v>79</v>
-      </c>
-      <c r="I16" s="0" t="s">
-        <v>80</v>
-      </c>
-      <c r="J16" s="0" t="n">
+        <v>106</v>
+      </c>
+      <c r="G16" s="0" t="n">
         <v>94588</v>
       </c>
-      <c r="K16" s="0" t="n">
+      <c r="H16" s="0" t="n">
         <v>36</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="17">
       <c r="A17" s="0" t="s">
-        <v>130</v>
+        <v>107</v>
       </c>
       <c r="B17" s="0" t="s">
         <v>26</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>131</v>
+        <v>108</v>
       </c>
       <c r="D17" s="0" t="n">
         <v>37.792976</v>
@@ -23727,33 +23434,24 @@
         <v>-122.396742</v>
       </c>
       <c r="F17" s="0" t="s">
-        <v>132</v>
-      </c>
-      <c r="G17" s="0" t="s">
-        <v>84</v>
-      </c>
-      <c r="H17" s="0" t="s">
-        <v>85</v>
-      </c>
-      <c r="I17" s="0" t="s">
-        <v>80</v>
-      </c>
-      <c r="J17" s="0" t="n">
+        <v>77</v>
+      </c>
+      <c r="G17" s="0" t="n">
         <v>94111</v>
       </c>
-      <c r="K17" s="0" t="n">
+      <c r="H17" s="0" t="n">
         <v>25</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="18">
       <c r="A18" s="0" t="s">
-        <v>133</v>
+        <v>109</v>
       </c>
       <c r="B18" s="0" t="s">
         <v>4</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>134</v>
+        <v>110</v>
       </c>
       <c r="D18" s="0" t="n">
         <v>37.925655</v>
@@ -23762,33 +23460,24 @@
         <v>-122.317269</v>
       </c>
       <c r="F18" s="0" t="s">
-        <v>135</v>
-      </c>
-      <c r="G18" s="0" t="s">
-        <v>136</v>
-      </c>
-      <c r="H18" s="0" t="s">
-        <v>116</v>
-      </c>
-      <c r="I18" s="0" t="s">
-        <v>80</v>
-      </c>
-      <c r="J18" s="0" t="n">
+        <v>111</v>
+      </c>
+      <c r="G18" s="0" t="n">
         <v>94530</v>
       </c>
-      <c r="K18" s="0" t="n">
+      <c r="H18" s="0" t="n">
         <v>1</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="19">
       <c r="A19" s="0" t="s">
-        <v>137</v>
+        <v>112</v>
       </c>
       <c r="B19" s="0" t="s">
         <v>5</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>138</v>
+        <v>113</v>
       </c>
       <c r="D19" s="0" t="n">
         <v>37.9030588</v>
@@ -23797,33 +23486,24 @@
         <v>-122.2992715</v>
       </c>
       <c r="F19" s="0" t="s">
-        <v>139</v>
-      </c>
-      <c r="G19" s="0" t="s">
-        <v>136</v>
-      </c>
-      <c r="H19" s="0" t="s">
-        <v>116</v>
-      </c>
-      <c r="I19" s="0" t="s">
-        <v>80</v>
-      </c>
-      <c r="J19" s="0" t="n">
+        <v>111</v>
+      </c>
+      <c r="G19" s="0" t="n">
         <v>94530</v>
       </c>
-      <c r="K19" s="0" t="n">
+      <c r="H19" s="0" t="n">
         <v>2</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="20">
       <c r="A20" s="0" t="s">
-        <v>140</v>
+        <v>114</v>
       </c>
       <c r="B20" s="0" t="s">
         <v>18</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>141</v>
+        <v>115</v>
       </c>
       <c r="D20" s="0" t="n">
         <v>37.557355</v>
@@ -23832,33 +23512,24 @@
         <v>-121.9764</v>
       </c>
       <c r="F20" s="0" t="s">
-        <v>142</v>
-      </c>
-      <c r="G20" s="0" t="s">
-        <v>140</v>
-      </c>
-      <c r="H20" s="0" t="s">
-        <v>79</v>
-      </c>
-      <c r="I20" s="0" t="s">
-        <v>80</v>
-      </c>
-      <c r="J20" s="0" t="n">
+        <v>114</v>
+      </c>
+      <c r="G20" s="0" t="n">
         <v>94536</v>
       </c>
-      <c r="K20" s="0" t="n">
+      <c r="H20" s="0" t="n">
         <v>17</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="21">
       <c r="A21" s="0" t="s">
-        <v>143</v>
+        <v>116</v>
       </c>
       <c r="B21" s="0" t="s">
         <v>11</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>144</v>
+        <v>117</v>
       </c>
       <c r="D21" s="0" t="n">
         <v>37.774963</v>
@@ -23867,33 +23538,24 @@
         <v>-122.224274</v>
       </c>
       <c r="F21" s="0" t="s">
-        <v>145</v>
-      </c>
-      <c r="G21" s="0" t="s">
-        <v>78</v>
-      </c>
-      <c r="H21" s="0" t="s">
-        <v>79</v>
-      </c>
-      <c r="I21" s="0" t="s">
-        <v>80</v>
-      </c>
-      <c r="J21" s="0" t="n">
+        <v>74</v>
+      </c>
+      <c r="G21" s="0" t="n">
         <v>94601</v>
       </c>
-      <c r="K21" s="0" t="n">
+      <c r="H21" s="0" t="n">
         <v>10</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="22">
       <c r="A22" s="0" t="s">
-        <v>146</v>
+        <v>118</v>
       </c>
       <c r="B22" s="0" t="s">
         <v>30</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>147</v>
+        <v>119</v>
       </c>
       <c r="D22" s="0" t="n">
         <v>37.732921</v>
@@ -23902,33 +23564,24 @@
         <v>-122.434092</v>
       </c>
       <c r="F22" s="0" t="s">
-        <v>148</v>
-      </c>
-      <c r="G22" s="0" t="s">
-        <v>84</v>
-      </c>
-      <c r="H22" s="0" t="s">
-        <v>85</v>
-      </c>
-      <c r="I22" s="0" t="s">
-        <v>80</v>
-      </c>
-      <c r="J22" s="0" t="n">
+        <v>77</v>
+      </c>
+      <c r="G22" s="0" t="n">
         <v>94131</v>
       </c>
-      <c r="K22" s="0" t="n">
+      <c r="H22" s="0" t="n">
         <v>31</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="23">
       <c r="A23" s="0" t="s">
-        <v>149</v>
+        <v>120</v>
       </c>
       <c r="B23" s="0" t="s">
         <v>15</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>150</v>
+        <v>121</v>
       </c>
       <c r="D23" s="0" t="n">
         <v>37.670399</v>
@@ -23937,33 +23590,24 @@
         <v>-122.087967</v>
       </c>
       <c r="F23" s="0" t="s">
-        <v>151</v>
-      </c>
-      <c r="G23" s="0" t="s">
-        <v>149</v>
-      </c>
-      <c r="H23" s="0" t="s">
-        <v>79</v>
-      </c>
-      <c r="I23" s="0" t="s">
-        <v>80</v>
-      </c>
-      <c r="J23" s="0" t="n">
+        <v>120</v>
+      </c>
+      <c r="G23" s="0" t="n">
         <v>94541</v>
       </c>
-      <c r="K23" s="0" t="n">
+      <c r="H23" s="0" t="n">
         <v>14</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="24">
       <c r="A24" s="0" t="s">
-        <v>152</v>
+        <v>122</v>
       </c>
       <c r="B24" s="0" t="s">
         <v>22</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>153</v>
+        <v>123</v>
       </c>
       <c r="D24" s="0" t="n">
         <v>37.893394</v>
@@ -23972,33 +23616,24 @@
         <v>-122.123801</v>
       </c>
       <c r="F24" s="0" t="s">
-        <v>154</v>
-      </c>
-      <c r="G24" s="0" t="s">
-        <v>152</v>
-      </c>
-      <c r="H24" s="0" t="s">
-        <v>116</v>
-      </c>
-      <c r="I24" s="0" t="s">
-        <v>80</v>
-      </c>
-      <c r="J24" s="0" t="n">
+        <v>122</v>
+      </c>
+      <c r="G24" s="0" t="n">
         <v>94549</v>
       </c>
-      <c r="K24" s="0" t="n">
+      <c r="H24" s="0" t="n">
         <v>21</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="25">
       <c r="A25" s="0" t="s">
-        <v>155</v>
+        <v>124</v>
       </c>
       <c r="B25" s="0" t="s">
         <v>10</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>156</v>
+        <v>125</v>
       </c>
       <c r="D25" s="0" t="n">
         <v>37.797484</v>
@@ -24007,33 +23642,24 @@
         <v>-122.265609</v>
       </c>
       <c r="F25" s="0" t="s">
-        <v>157</v>
-      </c>
-      <c r="G25" s="0" t="s">
-        <v>78</v>
-      </c>
-      <c r="H25" s="0" t="s">
-        <v>79</v>
-      </c>
-      <c r="I25" s="0" t="s">
-        <v>80</v>
-      </c>
-      <c r="J25" s="0" t="n">
+        <v>74</v>
+      </c>
+      <c r="G25" s="0" t="n">
         <v>94607</v>
       </c>
-      <c r="K25" s="0" t="n">
+      <c r="H25" s="0" t="n">
         <v>9</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="26">
       <c r="A26" s="0" t="s">
-        <v>158</v>
+        <v>126</v>
       </c>
       <c r="B26" s="0" t="s">
         <v>9</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>159</v>
+        <v>127</v>
       </c>
       <c r="D26" s="0" t="n">
         <v>37.828415</v>
@@ -24042,33 +23668,24 @@
         <v>-122.267227</v>
       </c>
       <c r="F26" s="0" t="s">
-        <v>160</v>
-      </c>
-      <c r="G26" s="0" t="s">
-        <v>78</v>
-      </c>
-      <c r="H26" s="0" t="s">
-        <v>79</v>
-      </c>
-      <c r="I26" s="0" t="s">
-        <v>80</v>
-      </c>
-      <c r="J26" s="0" t="n">
+        <v>74</v>
+      </c>
+      <c r="G26" s="0" t="n">
         <v>94609</v>
       </c>
-      <c r="K26" s="0" t="n">
+      <c r="H26" s="0" t="n">
         <v>6</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="27">
       <c r="A27" s="0" t="s">
-        <v>161</v>
+        <v>128</v>
       </c>
       <c r="B27" s="0" t="s">
         <v>41</v>
       </c>
       <c r="C27" s="0" t="s">
-        <v>162</v>
+        <v>129</v>
       </c>
       <c r="D27" s="0" t="n">
         <v>37.599787</v>
@@ -24077,33 +23694,24 @@
         <v>-122.38666</v>
       </c>
       <c r="F27" s="0" t="s">
-        <v>163</v>
-      </c>
-      <c r="G27" s="0" t="s">
-        <v>161</v>
-      </c>
-      <c r="H27" s="0" t="s">
-        <v>112</v>
-      </c>
-      <c r="I27" s="0" t="s">
-        <v>80</v>
-      </c>
-      <c r="J27" s="0" t="n">
+        <v>128</v>
+      </c>
+      <c r="G27" s="0" t="n">
         <v>94030</v>
       </c>
-      <c r="K27" s="0" t="n">
+      <c r="H27" s="0" t="n">
         <v>42</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="28">
       <c r="A28" s="0" t="s">
-        <v>164</v>
+        <v>130</v>
       </c>
       <c r="B28" s="0" t="s">
         <v>27</v>
       </c>
       <c r="C28" s="0" t="s">
-        <v>165</v>
+        <v>131</v>
       </c>
       <c r="D28" s="0" t="n">
         <v>37.789256</v>
@@ -24112,33 +23720,24 @@
         <v>-122.401407</v>
       </c>
       <c r="F28" s="0" t="s">
-        <v>166</v>
-      </c>
-      <c r="G28" s="0" t="s">
-        <v>84</v>
-      </c>
-      <c r="H28" s="0" t="s">
-        <v>85</v>
-      </c>
-      <c r="I28" s="0" t="s">
-        <v>80</v>
-      </c>
-      <c r="J28" s="0" t="n">
+        <v>77</v>
+      </c>
+      <c r="G28" s="0" t="n">
         <v>94104</v>
       </c>
-      <c r="K28" s="0" t="n">
+      <c r="H28" s="0" t="n">
         <v>26</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="29">
       <c r="A29" s="0" t="s">
-        <v>167</v>
+        <v>132</v>
       </c>
       <c r="B29" s="0" t="s">
         <v>6</v>
       </c>
       <c r="C29" s="0" t="s">
-        <v>168</v>
+        <v>133</v>
       </c>
       <c r="D29" s="0" t="n">
         <v>37.87404</v>
@@ -24147,33 +23746,24 @@
         <v>-122.283451</v>
       </c>
       <c r="F29" s="0" t="s">
-        <v>169</v>
-      </c>
-      <c r="G29" s="0" t="s">
-        <v>95</v>
-      </c>
-      <c r="H29" s="0" t="s">
-        <v>79</v>
-      </c>
-      <c r="I29" s="0" t="s">
-        <v>80</v>
-      </c>
-      <c r="J29" s="0" t="n">
+        <v>84</v>
+      </c>
+      <c r="G29" s="0" t="n">
         <v>94702</v>
       </c>
-      <c r="K29" s="0" t="n">
+      <c r="H29" s="0" t="n">
         <v>3</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="30">
       <c r="A30" s="0" t="s">
-        <v>170</v>
+        <v>134</v>
       </c>
       <c r="B30" s="0" t="s">
         <v>36</v>
       </c>
       <c r="C30" s="0" t="s">
-        <v>171</v>
+        <v>135</v>
       </c>
       <c r="D30" s="0" t="n">
         <v>38.003275</v>
@@ -24182,33 +23772,24 @@
         <v>-122.024597</v>
       </c>
       <c r="F30" s="0" t="s">
-        <v>172</v>
-      </c>
-      <c r="G30" s="0" t="s">
-        <v>113</v>
-      </c>
-      <c r="H30" s="0" t="s">
-        <v>116</v>
-      </c>
-      <c r="I30" s="0" t="s">
-        <v>80</v>
-      </c>
-      <c r="J30" s="0" t="n">
+        <v>96</v>
+      </c>
+      <c r="G30" s="0" t="n">
         <v>94520</v>
       </c>
-      <c r="K30" s="0" t="n">
+      <c r="H30" s="0" t="n">
         <v>37</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="31">
       <c r="A31" s="0" t="s">
-        <v>173</v>
+        <v>136</v>
       </c>
       <c r="B31" s="0" t="s">
         <v>23</v>
       </c>
       <c r="C31" s="0" t="s">
-        <v>174</v>
+        <v>137</v>
       </c>
       <c r="D31" s="0" t="n">
         <v>37.87836087</v>
@@ -24217,33 +23798,24 @@
         <v>-122.1837911</v>
       </c>
       <c r="F31" s="0" t="s">
-        <v>175</v>
-      </c>
-      <c r="G31" s="0" t="s">
-        <v>173</v>
-      </c>
-      <c r="H31" s="0" t="s">
-        <v>116</v>
-      </c>
-      <c r="I31" s="0" t="s">
-        <v>80</v>
-      </c>
-      <c r="J31" s="0" t="n">
+        <v>136</v>
+      </c>
+      <c r="G31" s="0" t="n">
         <v>94563</v>
       </c>
-      <c r="K31" s="0" t="n">
+      <c r="H31" s="0" t="n">
         <v>22</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="32">
       <c r="A32" s="0" t="s">
-        <v>176</v>
+        <v>138</v>
       </c>
       <c r="B32" s="0" t="s">
         <v>25</v>
       </c>
       <c r="C32" s="0" t="s">
-        <v>177</v>
+        <v>139</v>
       </c>
       <c r="D32" s="0" t="n">
         <v>37.80467476</v>
@@ -24252,33 +23824,24 @@
         <v>-122.2945822</v>
       </c>
       <c r="F32" s="0" t="s">
-        <v>178</v>
-      </c>
-      <c r="G32" s="0" t="s">
-        <v>78</v>
-      </c>
-      <c r="H32" s="0" t="s">
-        <v>79</v>
-      </c>
-      <c r="I32" s="0" t="s">
-        <v>80</v>
-      </c>
-      <c r="J32" s="0" t="n">
+        <v>74</v>
+      </c>
+      <c r="G32" s="0" t="n">
         <v>94607</v>
       </c>
-      <c r="K32" s="0" t="n">
+      <c r="H32" s="0" t="n">
         <v>24</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="33">
       <c r="A33" s="0" t="s">
-        <v>179</v>
+        <v>140</v>
       </c>
       <c r="B33" s="0" t="s">
         <v>20</v>
       </c>
       <c r="C33" s="0" t="s">
-        <v>180</v>
+        <v>141</v>
       </c>
       <c r="D33" s="0" t="n">
         <v>37.928403</v>
@@ -24287,33 +23850,24 @@
         <v>-122.056013</v>
       </c>
       <c r="F33" s="0" t="s">
-        <v>181</v>
-      </c>
-      <c r="G33" s="0" t="s">
-        <v>182</v>
-      </c>
-      <c r="H33" s="0" t="s">
-        <v>116</v>
-      </c>
-      <c r="I33" s="0" t="s">
-        <v>80</v>
-      </c>
-      <c r="J33" s="0" t="n">
+        <v>142</v>
+      </c>
+      <c r="G33" s="0" t="n">
         <v>94597</v>
       </c>
-      <c r="K33" s="0" t="n">
+      <c r="H33" s="0" t="n">
         <v>19</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="34">
       <c r="A34" s="0" t="s">
-        <v>183</v>
+        <v>143</v>
       </c>
       <c r="B34" s="0" t="s">
         <v>28</v>
       </c>
       <c r="C34" s="0" t="s">
-        <v>184</v>
+        <v>144</v>
       </c>
       <c r="D34" s="0" t="n">
         <v>37.784991</v>
@@ -24322,33 +23876,24 @@
         <v>-122.406857</v>
       </c>
       <c r="F34" s="0" t="s">
-        <v>185</v>
-      </c>
-      <c r="G34" s="0" t="s">
-        <v>84</v>
-      </c>
-      <c r="H34" s="0" t="s">
-        <v>85</v>
-      </c>
-      <c r="I34" s="0" t="s">
-        <v>80</v>
-      </c>
-      <c r="J34" s="0" t="n">
+        <v>77</v>
+      </c>
+      <c r="G34" s="0" t="n">
         <v>94102</v>
       </c>
-      <c r="K34" s="0" t="n">
+      <c r="H34" s="0" t="n">
         <v>27</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="35">
       <c r="A35" s="0" t="s">
-        <v>186</v>
+        <v>145</v>
       </c>
       <c r="B35" s="0" t="s">
         <v>3</v>
       </c>
       <c r="C35" s="0" t="s">
-        <v>187</v>
+        <v>146</v>
       </c>
       <c r="D35" s="0" t="n">
         <v>37.936887</v>
@@ -24357,33 +23902,24 @@
         <v>-122.353165</v>
       </c>
       <c r="F35" s="0" t="s">
-        <v>188</v>
-      </c>
-      <c r="G35" s="0" t="s">
-        <v>186</v>
-      </c>
-      <c r="H35" s="0" t="s">
-        <v>116</v>
-      </c>
-      <c r="I35" s="0" t="s">
-        <v>80</v>
-      </c>
-      <c r="J35" s="0" t="n">
+        <v>145</v>
+      </c>
+      <c r="G35" s="0" t="n">
         <v>94801</v>
       </c>
-      <c r="K35" s="0" t="n">
+      <c r="H35" s="0" t="n">
         <v>0</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="36">
       <c r="A36" s="0" t="s">
-        <v>189</v>
+        <v>147</v>
       </c>
       <c r="B36" s="0" t="s">
         <v>24</v>
       </c>
       <c r="C36" s="0" t="s">
-        <v>190</v>
+        <v>148</v>
       </c>
       <c r="D36" s="0" t="n">
         <v>37.844601</v>
@@ -24392,33 +23928,24 @@
         <v>-122.251793</v>
       </c>
       <c r="F36" s="0" t="s">
-        <v>191</v>
-      </c>
-      <c r="G36" s="0" t="s">
-        <v>78</v>
-      </c>
-      <c r="H36" s="0" t="s">
-        <v>79</v>
-      </c>
-      <c r="I36" s="0" t="s">
-        <v>80</v>
-      </c>
-      <c r="J36" s="0" t="n">
+        <v>74</v>
+      </c>
+      <c r="G36" s="0" t="n">
         <v>94618</v>
       </c>
-      <c r="K36" s="0" t="n">
+      <c r="H36" s="0" t="n">
         <v>23</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="37">
       <c r="A37" s="0" t="s">
-        <v>192</v>
+        <v>149</v>
       </c>
       <c r="B37" s="0" t="s">
         <v>39</v>
       </c>
       <c r="C37" s="0" t="s">
-        <v>193</v>
+        <v>150</v>
       </c>
       <c r="D37" s="0" t="n">
         <v>37.637753</v>
@@ -24427,33 +23954,24 @@
         <v>-122.416038</v>
       </c>
       <c r="F37" s="0" t="s">
-        <v>194</v>
-      </c>
-      <c r="G37" s="0" t="s">
-        <v>192</v>
-      </c>
-      <c r="H37" s="0" t="s">
-        <v>112</v>
-      </c>
-      <c r="I37" s="0" t="s">
-        <v>80</v>
-      </c>
-      <c r="J37" s="0" t="n">
+        <v>149</v>
+      </c>
+      <c r="G37" s="0" t="n">
         <v>94066</v>
       </c>
-      <c r="K37" s="0" t="n">
+      <c r="H37" s="0" t="n">
         <v>40</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="38">
       <c r="A38" s="0" t="s">
-        <v>195</v>
+        <v>151</v>
       </c>
       <c r="B38" s="0" t="s">
         <v>16</v>
       </c>
       <c r="C38" s="0" t="s">
-        <v>196</v>
+        <v>152</v>
       </c>
       <c r="D38" s="0" t="n">
         <v>37.63479954</v>
@@ -24462,33 +23980,24 @@
         <v>-122.0575506</v>
       </c>
       <c r="F38" s="0" t="s">
-        <v>197</v>
-      </c>
-      <c r="G38" s="0" t="s">
-        <v>149</v>
-      </c>
-      <c r="H38" s="0" t="s">
-        <v>79</v>
-      </c>
-      <c r="I38" s="0" t="s">
-        <v>80</v>
-      </c>
-      <c r="J38" s="0" t="n">
+        <v>120</v>
+      </c>
+      <c r="G38" s="0" t="n">
         <v>94544</v>
       </c>
-      <c r="K38" s="0" t="n">
+      <c r="H38" s="0" t="n">
         <v>15</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="39">
       <c r="A39" s="0" t="s">
-        <v>99</v>
+        <v>87</v>
       </c>
       <c r="B39" s="0" t="s">
         <v>13</v>
       </c>
       <c r="C39" s="0" t="s">
-        <v>198</v>
+        <v>153</v>
       </c>
       <c r="D39" s="0" t="n">
         <v>37.72261921</v>
@@ -24497,27 +24006,18 @@
         <v>-122.1613112</v>
       </c>
       <c r="F39" s="0" t="s">
-        <v>199</v>
-      </c>
-      <c r="G39" s="0" t="s">
-        <v>99</v>
-      </c>
-      <c r="H39" s="0" t="s">
-        <v>79</v>
-      </c>
-      <c r="I39" s="0" t="s">
-        <v>80</v>
-      </c>
-      <c r="J39" s="0" t="n">
+        <v>87</v>
+      </c>
+      <c r="G39" s="0" t="n">
         <v>94577</v>
       </c>
-      <c r="K39" s="0" t="n">
+      <c r="H39" s="0" t="n">
         <v>12</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="40">
       <c r="A40" s="0" t="s">
-        <v>200</v>
+        <v>154</v>
       </c>
       <c r="B40" s="0" t="s">
         <v>40</v>
@@ -24532,33 +24032,24 @@
         <v>-122.392612</v>
       </c>
       <c r="F40" s="0" t="s">
-        <v>201</v>
-      </c>
-      <c r="G40" s="0" t="s">
-        <v>200</v>
-      </c>
-      <c r="H40" s="0" t="s">
-        <v>112</v>
-      </c>
-      <c r="I40" s="0" t="s">
-        <v>80</v>
-      </c>
-      <c r="J40" s="0" t="n">
+        <v>154</v>
+      </c>
+      <c r="G40" s="0" t="n">
         <v>94128</v>
       </c>
-      <c r="K40" s="0" t="n">
+      <c r="H40" s="0" t="n">
         <v>41</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="41">
       <c r="A41" s="0" t="s">
-        <v>202</v>
+        <v>155</v>
       </c>
       <c r="B41" s="0" t="s">
         <v>38</v>
       </c>
       <c r="C41" s="0" t="s">
-        <v>203</v>
+        <v>156</v>
       </c>
       <c r="D41" s="0" t="n">
         <v>37.664174</v>
@@ -24567,33 +24058,24 @@
         <v>-122.444116</v>
       </c>
       <c r="F41" s="0" t="s">
-        <v>204</v>
-      </c>
-      <c r="G41" s="0" t="s">
-        <v>202</v>
-      </c>
-      <c r="H41" s="0" t="s">
-        <v>112</v>
-      </c>
-      <c r="I41" s="0" t="s">
-        <v>80</v>
-      </c>
-      <c r="J41" s="0" t="n">
+        <v>155</v>
+      </c>
+      <c r="G41" s="0" t="n">
         <v>94080</v>
       </c>
-      <c r="K41" s="0" t="n">
+      <c r="H41" s="0" t="n">
         <v>39</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="42">
       <c r="A42" s="0" t="s">
-        <v>205</v>
+        <v>157</v>
       </c>
       <c r="B42" s="0" t="s">
         <v>17</v>
       </c>
       <c r="C42" s="0" t="s">
-        <v>206</v>
+        <v>158</v>
       </c>
       <c r="D42" s="0" t="n">
         <v>37.591208</v>
@@ -24602,33 +24084,24 @@
         <v>-122.017867</v>
       </c>
       <c r="F42" s="0" t="s">
-        <v>207</v>
-      </c>
-      <c r="G42" s="0" t="s">
-        <v>205</v>
-      </c>
-      <c r="H42" s="0" t="s">
-        <v>79</v>
-      </c>
-      <c r="I42" s="0" t="s">
-        <v>80</v>
-      </c>
-      <c r="J42" s="0" t="n">
+        <v>157</v>
+      </c>
+      <c r="G42" s="0" t="n">
         <v>94587</v>
       </c>
-      <c r="K42" s="0" t="n">
+      <c r="H42" s="0" t="n">
         <v>16</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="43">
       <c r="A43" s="0" t="s">
-        <v>182</v>
+        <v>142</v>
       </c>
       <c r="B43" s="0" t="s">
         <v>21</v>
       </c>
       <c r="C43" s="0" t="s">
-        <v>208</v>
+        <v>159</v>
       </c>
       <c r="D43" s="0" t="n">
         <v>37.905628</v>
@@ -24637,33 +24110,24 @@
         <v>-122.067423</v>
       </c>
       <c r="F43" s="0" t="s">
-        <v>209</v>
-      </c>
-      <c r="G43" s="0" t="s">
-        <v>182</v>
-      </c>
-      <c r="H43" s="0" t="s">
-        <v>116</v>
-      </c>
-      <c r="I43" s="0" t="s">
-        <v>80</v>
-      </c>
-      <c r="J43" s="0" t="n">
+        <v>142</v>
+      </c>
+      <c r="G43" s="0" t="n">
         <v>94596</v>
       </c>
-      <c r="K43" s="0" t="n">
+      <c r="H43" s="0" t="n">
         <v>20</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="44">
       <c r="A44" s="0" t="s">
-        <v>210</v>
+        <v>160</v>
       </c>
       <c r="B44" s="0" t="s">
         <v>42</v>
       </c>
       <c r="C44" s="0" t="s">
-        <v>211</v>
+        <v>161</v>
       </c>
       <c r="D44" s="0" t="n">
         <v>37.699759</v>
@@ -24672,33 +24136,24 @@
         <v>-121.928099</v>
       </c>
       <c r="F44" s="0" t="s">
-        <v>212</v>
-      </c>
-      <c r="G44" s="0" t="s">
-        <v>213</v>
-      </c>
-      <c r="H44" s="0" t="s">
-        <v>79</v>
-      </c>
-      <c r="I44" s="0" t="s">
-        <v>80</v>
-      </c>
-      <c r="J44" s="0" t="n">
+        <v>162</v>
+      </c>
+      <c r="G44" s="0" t="n">
         <v>94568</v>
       </c>
-      <c r="K44" s="0" t="n">
+      <c r="H44" s="0" t="n">
         <v>43</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="45">
       <c r="A45" s="0" t="s">
-        <v>214</v>
+        <v>163</v>
       </c>
       <c r="B45" s="0" t="s">
         <v>37</v>
       </c>
       <c r="C45" s="0" t="s">
-        <v>215</v>
+        <v>164</v>
       </c>
       <c r="D45" s="0" t="n">
         <v>38.018914</v>
@@ -24707,21 +24162,12 @@
         <v>-121.945154</v>
       </c>
       <c r="F45" s="0" t="s">
-        <v>216</v>
-      </c>
-      <c r="G45" s="0" t="s">
-        <v>217</v>
-      </c>
-      <c r="H45" s="0" t="s">
-        <v>116</v>
-      </c>
-      <c r="I45" s="0" t="s">
-        <v>80</v>
-      </c>
-      <c r="J45" s="0" t="n">
+        <v>165</v>
+      </c>
+      <c r="G45" s="0" t="n">
         <v>94565</v>
       </c>
-      <c r="K45" s="0" t="n">
+      <c r="H45" s="0" t="n">
         <v>38</v>
       </c>
     </row>
@@ -24748,10 +24194,10 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5764705882353"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.6313725490196"/>
   </cols>
   <sheetData>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="1">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="1">
       <c r="A1" s="5" t="n">
         <v>12</v>
       </c>
@@ -24763,7 +24209,7 @@
         <v>8</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="2">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="2">
       <c r="A2" s="5" t="n">
         <v>16</v>
       </c>
@@ -24775,7 +24221,7 @@
         <v>29</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="3">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="3">
       <c r="A3" s="5" t="n">
         <v>19</v>
       </c>
@@ -24787,7 +24233,7 @@
         <v>7</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="4">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="4">
       <c r="A4" s="5" t="n">
         <v>24</v>
       </c>
@@ -24799,7 +24245,7 @@
         <v>30</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="5">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="5">
       <c r="A5" s="5" t="s">
         <v>8</v>
       </c>
@@ -24811,7 +24257,7 @@
         <v>5</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="6">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="6">
       <c r="A6" s="5" t="s">
         <v>14</v>
       </c>
@@ -24823,7 +24269,7 @@
         <v>13</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="7">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="7">
       <c r="A7" s="5" t="s">
         <v>7</v>
       </c>
@@ -24835,7 +24281,7 @@
         <v>4</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="8">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="8">
       <c r="A8" s="5" t="s">
         <v>31</v>
       </c>
@@ -24847,7 +24293,7 @@
         <v>32</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="9">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="9">
       <c r="A9" s="5" t="s">
         <v>29</v>
       </c>
@@ -24859,7 +24305,7 @@
         <v>28</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="10">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="10">
       <c r="A10" s="5" t="s">
         <v>12</v>
       </c>
@@ -24871,7 +24317,7 @@
         <v>11</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="11">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="11">
       <c r="A11" s="5" t="s">
         <v>33</v>
       </c>
@@ -24883,7 +24329,7 @@
         <v>34</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="12">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="12">
       <c r="A12" s="5" t="s">
         <v>19</v>
       </c>
@@ -24895,7 +24341,7 @@
         <v>18</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="13">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="13">
       <c r="A13" s="5" t="s">
         <v>34</v>
       </c>
@@ -24907,7 +24353,7 @@
         <v>35</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="14">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="14">
       <c r="A14" s="5" t="s">
         <v>32</v>
       </c>
@@ -24919,7 +24365,7 @@
         <v>33</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="15">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="15">
       <c r="A15" s="5" t="s">
         <v>35</v>
       </c>
@@ -24931,7 +24377,7 @@
         <v>36</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="16">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="16">
       <c r="A16" s="5" t="s">
         <v>26</v>
       </c>
@@ -24943,7 +24389,7 @@
         <v>25</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="17">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="17">
       <c r="A17" s="5" t="s">
         <v>4</v>
       </c>
@@ -24955,7 +24401,7 @@
         <v>1</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="18">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="18">
       <c r="A18" s="5" t="s">
         <v>5</v>
       </c>
@@ -24967,7 +24413,7 @@
         <v>2</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="19">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="19">
       <c r="A19" s="5" t="s">
         <v>18</v>
       </c>
@@ -24979,7 +24425,7 @@
         <v>17</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="20">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="20">
       <c r="A20" s="5" t="s">
         <v>11</v>
       </c>
@@ -24991,7 +24437,7 @@
         <v>10</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="21">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="21">
       <c r="A21" s="5" t="s">
         <v>30</v>
       </c>
@@ -25003,7 +24449,7 @@
         <v>31</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="22">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="22">
       <c r="A22" s="5" t="s">
         <v>15</v>
       </c>
@@ -25015,7 +24461,7 @@
         <v>14</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="23">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="23">
       <c r="A23" s="5" t="s">
         <v>22</v>
       </c>
@@ -25027,7 +24473,7 @@
         <v>21</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="24">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="24">
       <c r="A24" s="5" t="s">
         <v>10</v>
       </c>
@@ -25039,7 +24485,7 @@
         <v>9</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="25">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="25">
       <c r="A25" s="5" t="s">
         <v>9</v>
       </c>
@@ -25051,7 +24497,7 @@
         <v>6</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="26">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="26">
       <c r="A26" s="5" t="s">
         <v>41</v>
       </c>
@@ -25063,7 +24509,7 @@
         <v>42</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="27">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="27">
       <c r="A27" s="5" t="s">
         <v>27</v>
       </c>
@@ -25075,7 +24521,7 @@
         <v>26</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="28">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="28">
       <c r="A28" s="5" t="s">
         <v>6</v>
       </c>
@@ -25087,7 +24533,7 @@
         <v>3</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="29">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="29">
       <c r="A29" s="5" t="s">
         <v>36</v>
       </c>
@@ -25099,7 +24545,7 @@
         <v>37</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="30">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="30">
       <c r="A30" s="5" t="s">
         <v>23</v>
       </c>
@@ -25111,7 +24557,7 @@
         <v>22</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="31">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="31">
       <c r="A31" s="5" t="s">
         <v>25</v>
       </c>
@@ -25123,7 +24569,7 @@
         <v>24</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="32">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="32">
       <c r="A32" s="5" t="s">
         <v>20</v>
       </c>
@@ -25135,7 +24581,7 @@
         <v>19</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="33">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="33">
       <c r="A33" s="5" t="s">
         <v>28</v>
       </c>
@@ -25147,7 +24593,7 @@
         <v>27</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="34">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="34">
       <c r="A34" s="5" t="s">
         <v>3</v>
       </c>
@@ -25159,7 +24605,7 @@
         <v>0</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="35">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="35">
       <c r="A35" s="5" t="s">
         <v>24</v>
       </c>
@@ -25171,7 +24617,7 @@
         <v>23</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="36">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="36">
       <c r="A36" s="5" t="s">
         <v>39</v>
       </c>
@@ -25183,7 +24629,7 @@
         <v>40</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="37">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="37">
       <c r="A37" s="5" t="s">
         <v>16</v>
       </c>
@@ -25195,7 +24641,7 @@
         <v>15</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="38">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="38">
       <c r="A38" s="5" t="s">
         <v>13</v>
       </c>
@@ -25207,7 +24653,7 @@
         <v>12</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="39">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="39">
       <c r="A39" s="5" t="s">
         <v>40</v>
       </c>
@@ -25219,7 +24665,7 @@
         <v>41</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="40">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="40">
       <c r="A40" s="5" t="s">
         <v>38</v>
       </c>
@@ -25231,7 +24677,7 @@
         <v>39</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="41">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="41">
       <c r="A41" s="5" t="s">
         <v>17</v>
       </c>
@@ -25243,7 +24689,7 @@
         <v>16</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="42">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="42">
       <c r="A42" s="5" t="s">
         <v>21</v>
       </c>
@@ -25255,7 +24701,7 @@
         <v>20</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="43">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="43">
       <c r="A43" s="5" t="s">
         <v>42</v>
       </c>
@@ -25267,7 +24713,7 @@
         <v>43</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="44">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="44">
       <c r="A44" s="5" t="s">
         <v>37</v>
       </c>

</xml_diff>